<commit_message>
add answers for enterprise lab.
</commit_message>
<xml_diff>
--- a/resources/tools/YARNCalcs.xlsx
+++ b/resources/tools/YARNCalcs.xlsx
@@ -606,7 +606,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -752,8 +752,8 @@
         <v>17</v>
       </c>
       <c r="F9" s="11">
-        <f>PRODUCT(F2,1024)</f>
-        <v>16384</v>
+        <f>F3</f>
+        <v>119808</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>